<commit_message>
Added to section 5 of SRS document
</commit_message>
<xml_diff>
--- a/Documents/Deliverable_1/CSwap_Deliverable_1_SprintBacklog_1.xlsx
+++ b/Documents/Deliverable_1/CSwap_Deliverable_1_SprintBacklog_1.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/landonthibodeau/git/COS420_Project/Documents/Deliverable_1/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{E52D378F-FE22-B942-BC85-D60202BA1200}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{440C06BB-B8D5-7140-9038-468C0D4818EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6540" yWindow="4280" windowWidth="28040" windowHeight="17440" xr2:uid="{49D0CED5-A062-EC43-94BD-79A001146B34}"/>
+    <workbookView xWindow="0" yWindow="880" windowWidth="20560" windowHeight="25700" xr2:uid="{49D0CED5-A062-EC43-94BD-79A001146B34}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sprint 1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sprint 2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -388,4 +389,16 @@
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ADAF5FEC-D2F5-EA48-B9F9-F3BA054FB78A}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>